<commit_message>
added admin page visible to only admins also added aprove/reject functionality
</commit_message>
<xml_diff>
--- a/server/items.xlsx
+++ b/server/items.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -433,6 +433,9 @@
       <c r="J1" t="str">
         <v>ReservedBy</v>
       </c>
+      <c r="K1" t="str">
+        <v>Approved</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -646,9 +649,102 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>test</v>
+      </c>
+      <c r="C9" t="str">
+        <v>test</v>
+      </c>
+      <c r="D9" t="str">
+        <v>other</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Excellent</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Taken</v>
+      </c>
+      <c r="G9" t="str">
+        <v>admin.mike@lsu.edu</v>
+      </c>
+      <c r="H9" t="str">
+        <v>photo-1763865475041-04mpl.jpg</v>
+      </c>
+      <c r="I9" t="str">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>admin test</v>
+      </c>
+      <c r="C10" t="str">
+        <v>This is a test to see if the admin can aprove</v>
+      </c>
+      <c r="D10" t="str">
+        <v>other</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Poor</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Available</v>
+      </c>
+      <c r="G10" t="str">
+        <v>admin.mike@lsu.edu</v>
+      </c>
+      <c r="H10" t="str">
+        <v>photo-1763868107950-0kdjg.jpg</v>
+      </c>
+      <c r="I10" t="str">
+        <v>9</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Lamp</v>
+      </c>
+      <c r="C11" t="str">
+        <v>A stock image of a lamp</v>
+      </c>
+      <c r="D11" t="str">
+        <v>furniture</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Excellent</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Available</v>
+      </c>
+      <c r="G11" t="str">
+        <v>alice@lsu.edu</v>
+      </c>
+      <c r="H11" t="str">
+        <v>photo-1763869213903-li17i.jpg</v>
+      </c>
+      <c r="I11" t="str">
+        <v>10</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added reject page where only  admins can type a reason for rejecting an item
</commit_message>
<xml_diff>
--- a/server/items.xlsx
+++ b/server/items.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -431,10 +431,10 @@
         <v>ImageFolder</v>
       </c>
       <c r="J1" t="str">
+        <v>Approved</v>
+      </c>
+      <c r="K1" t="str">
         <v>ReservedBy</v>
-      </c>
-      <c r="K1" t="str">
-        <v>Approved</v>
       </c>
     </row>
     <row r="2">
@@ -463,6 +463,9 @@
         <v>calc-book.jpg</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -494,7 +497,10 @@
       <c r="I3">
         <v>2</v>
       </c>
-      <c r="J3" t="str">
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="str">
         <v>alice@college.edu</v>
       </c>
     </row>
@@ -526,6 +532,9 @@
       <c r="I4" t="str">
         <v>3</v>
       </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -555,7 +564,10 @@
       <c r="I5" t="str">
         <v>4</v>
       </c>
-      <c r="J5" t="str">
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="str">
         <v>alice@lsu.edu</v>
       </c>
     </row>
@@ -587,7 +599,10 @@
       <c r="I6" t="str">
         <v>5</v>
       </c>
-      <c r="J6" t="str">
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="str">
         <v>alice@lsu.edu</v>
       </c>
     </row>
@@ -619,6 +634,9 @@
       <c r="I7" t="str">
         <v>6</v>
       </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -648,103 +666,13 @@
       <c r="I8" t="str">
         <v>7</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="str">
-        <v>test</v>
-      </c>
-      <c r="C9" t="str">
-        <v>test</v>
-      </c>
-      <c r="D9" t="str">
-        <v>other</v>
-      </c>
-      <c r="E9" t="str">
-        <v>Excellent</v>
-      </c>
-      <c r="F9" t="str">
-        <v>Taken</v>
-      </c>
-      <c r="G9" t="str">
-        <v>admin.mike@lsu.edu</v>
-      </c>
-      <c r="H9" t="str">
-        <v>photo-1763865475041-04mpl.jpg</v>
-      </c>
-      <c r="I9" t="str">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="str">
-        <v>admin test</v>
-      </c>
-      <c r="C10" t="str">
-        <v>This is a test to see if the admin can aprove</v>
-      </c>
-      <c r="D10" t="str">
-        <v>other</v>
-      </c>
-      <c r="E10" t="str">
-        <v>Poor</v>
-      </c>
-      <c r="F10" t="str">
-        <v>Available</v>
-      </c>
-      <c r="G10" t="str">
-        <v>admin.mike@lsu.edu</v>
-      </c>
-      <c r="H10" t="str">
-        <v>photo-1763868107950-0kdjg.jpg</v>
-      </c>
-      <c r="I10" t="str">
-        <v>9</v>
-      </c>
-      <c r="K10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Lamp</v>
-      </c>
-      <c r="C11" t="str">
-        <v>A stock image of a lamp</v>
-      </c>
-      <c r="D11" t="str">
-        <v>furniture</v>
-      </c>
-      <c r="E11" t="str">
-        <v>Excellent</v>
-      </c>
-      <c r="F11" t="str">
-        <v>Available</v>
-      </c>
-      <c r="G11" t="str">
-        <v>alice@lsu.edu</v>
-      </c>
-      <c r="H11" t="str">
-        <v>photo-1763869213903-li17i.jpg</v>
-      </c>
-      <c r="I11" t="str">
-        <v>10</v>
-      </c>
-      <c r="K11" t="b">
+      <c r="J8" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more unit tests, Integration tests and System tests with some changes to donating fields being validated. Added some users and an admin.
</commit_message>
<xml_diff>
--- a/server/items.xlsx
+++ b/server/items.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -439,31 +439,31 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="str">
-        <v>Calculus I Textbook</v>
+        <v>Desk Lamp</v>
       </c>
       <c r="C2" t="str">
-        <v>10th ed, like new</v>
+        <v>Working well, I have just use for six months</v>
       </c>
       <c r="D2" t="str">
-        <v>textbooks</v>
+        <v>electronics</v>
       </c>
       <c r="E2" t="str">
         <v>Excellent</v>
       </c>
       <c r="F2" t="str">
-        <v>Taken</v>
+        <v>Available</v>
       </c>
       <c r="G2" t="str">
         <v>alice@college.edu</v>
       </c>
       <c r="H2" t="str">
-        <v>calc-book.jpg</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
+        <v>photo-1762821083439.jpg,photo-1762821083443.jpeg</v>
+      </c>
+      <c r="I2" t="str">
+        <v>3</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
@@ -471,153 +471,153 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="str">
-        <v>IKEA Desk Chair</v>
+        <v>Microwave</v>
       </c>
       <c r="C3" t="str">
-        <v>Black, good condition</v>
+        <v>I have been using it for two years and still working good</v>
       </c>
       <c r="D3" t="str">
-        <v>furniture</v>
+        <v>electronics</v>
       </c>
       <c r="E3" t="str">
-        <v>Good</v>
+        <v>Fair</v>
       </c>
       <c r="F3" t="str">
         <v>Reserved</v>
       </c>
       <c r="G3" t="str">
-        <v>prof.bob@college.edu</v>
+        <v>alice@college.edu</v>
       </c>
       <c r="H3" t="str">
-        <v>chair.jpg</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
+        <v>photo-1762821913662-bqmb4.jpg</v>
+      </c>
+      <c r="I3" t="str">
+        <v>4</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
       </c>
       <c r="K3" t="str">
-        <v>alice@college.edu</v>
+        <v>alice@lsu.edu</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" t="str">
-        <v>Desk Lamp</v>
+        <v>English Text Book</v>
       </c>
       <c r="C4" t="str">
-        <v>Working well, I have just use for six months</v>
+        <v>I read the book, and it was too good</v>
       </c>
       <c r="D4" t="str">
-        <v>electronics</v>
+        <v>textbooks</v>
       </c>
       <c r="E4" t="str">
         <v>Excellent</v>
       </c>
       <c r="F4" t="str">
-        <v>Available</v>
+        <v>Reserved</v>
       </c>
       <c r="G4" t="str">
-        <v>alice@college.edu</v>
+        <v>prof.bob@college.edu</v>
       </c>
       <c r="H4" t="str">
-        <v>photo-1762821083439.jpg,photo-1762821083443.jpeg</v>
+        <v>photo-1762825185346-6re99.jpg</v>
       </c>
       <c r="I4" t="str">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
       </c>
+      <c r="K4" t="str">
+        <v>alice@lsu.edu</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" t="str">
-        <v>Microwave</v>
+        <v>Watch</v>
       </c>
       <c r="C5" t="str">
-        <v>I have been using it for two years and still working good</v>
+        <v>I have been using it for like seven months and it still working</v>
       </c>
       <c r="D5" t="str">
         <v>electronics</v>
       </c>
       <c r="E5" t="str">
-        <v>Fair</v>
+        <v>Good</v>
       </c>
       <c r="F5" t="str">
-        <v>Reserved</v>
+        <v>Available</v>
       </c>
       <c r="G5" t="str">
         <v>alice@college.edu</v>
       </c>
       <c r="H5" t="str">
-        <v>photo-1762821913662-bqmb4.jpg</v>
+        <v>default.jpg</v>
       </c>
       <c r="I5" t="str">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J5" t="b">
         <v>1</v>
       </c>
-      <c r="K5" t="str">
-        <v>alice@lsu.edu</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" t="str">
-        <v>English Text Book</v>
+        <v>System Test Calculus Textbook</v>
       </c>
       <c r="C6" t="str">
-        <v>I read the book, and it was too good</v>
+        <v>Advanced Calculus - hardcover</v>
       </c>
       <c r="D6" t="str">
-        <v>textbooks</v>
+        <v>Books</v>
       </c>
       <c r="E6" t="str">
         <v>Excellent</v>
       </c>
       <c r="F6" t="str">
-        <v>Reserved</v>
+        <v>Taken</v>
       </c>
       <c r="G6" t="str">
-        <v>prof.bob@college.edu</v>
+        <v>alice@lsu.edu</v>
       </c>
       <c r="H6" t="str">
-        <v>photo-1762825185346-6re99.jpg</v>
+        <v>default.jpg</v>
       </c>
       <c r="I6" t="str">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
       </c>
       <c r="K6" t="str">
-        <v>alice@lsu.edu</v>
+        <v>james@lsu.edu</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="str">
-        <v>Watch</v>
+        <v>System Test Monitor</v>
       </c>
       <c r="C7" t="str">
-        <v>I have been using it for like seven months and it still working</v>
+        <v>27 inch LED monitor, works perfectly</v>
       </c>
       <c r="D7" t="str">
-        <v>electronics</v>
+        <v>Electronics</v>
       </c>
       <c r="E7" t="str">
         <v>Good</v>
@@ -626,13 +626,13 @@
         <v>Available</v>
       </c>
       <c r="G7" t="str">
-        <v>alice@college.edu</v>
+        <v>carlos@lsu.edu</v>
       </c>
       <c r="H7" t="str">
         <v>default.jpg</v>
       </c>
       <c r="I7" t="str">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -640,39 +640,106 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" t="str">
-        <v>book</v>
+        <v>System Test Bookshelf</v>
       </c>
       <c r="C8" t="str">
-        <v>this is a test book</v>
+        <v>Wooden bookshelf, 5 shelves</v>
       </c>
       <c r="D8" t="str">
-        <v>textbooks</v>
+        <v>Furniture</v>
       </c>
       <c r="E8" t="str">
+        <v>Good</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Pending Aproval</v>
+      </c>
+      <c r="G8" t="str">
+        <v>sarah@lsu.edu</v>
+      </c>
+      <c r="H8" t="str">
+        <v>default.jpg</v>
+      </c>
+      <c r="I8" t="str">
+        <v>9</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Integrity Test Item</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Testing data integrity</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Books</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Good</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Pending Aproval</v>
+      </c>
+      <c r="G9" t="str">
+        <v>james@lsu.edu</v>
+      </c>
+      <c r="H9" t="str">
+        <v>default.jpg</v>
+      </c>
+      <c r="I9" t="str">
+        <v>10</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Reservation Test Item</v>
+      </c>
+      <c r="C10" t="str">
+        <v>For reservation testing</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="E10" t="str">
         <v>Excellent</v>
       </c>
-      <c r="F8" t="str">
-        <v>Available</v>
-      </c>
-      <c r="G8" t="str">
-        <v>alice@lsu.edu</v>
-      </c>
-      <c r="H8" t="str">
-        <v>photo-1763270863374-7dpr8.jpg</v>
-      </c>
-      <c r="I8" t="str">
-        <v>7</v>
-      </c>
-      <c r="J8" t="b">
+      <c r="F10" t="str">
+        <v>Reserved</v>
+      </c>
+      <c r="G10" t="str">
+        <v>carlos@lsu.edu</v>
+      </c>
+      <c r="H10" t="str">
+        <v>default.jpg</v>
+      </c>
+      <c r="I10" t="str">
+        <v>11</v>
+      </c>
+      <c r="J10" t="b">
         <v>1</v>
+      </c>
+      <c r="K10" t="str">
+        <v>sarah@lsu.edu</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>